<commit_message>
Compiled phenotype-cnv association results in spreadsheet
</commit_message>
<xml_diff>
--- a/Phenotype_cnv_associations/Combined_results.xlsx
+++ b/Phenotype_cnv_associations/Combined_results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10960" yWindow="3580" windowWidth="25600" windowHeight="15600" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="7880" yWindow="2160" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="height_simple" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="169" formatCode="0.0000"/>
-    <numFmt numFmtId="170" formatCode="0.000"/>
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -109,7 +108,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -141,15 +140,44 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -165,6 +193,21 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -180,6 +223,21 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -458,7 +516,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C10"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -588,7 +646,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C10"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -705,6 +763,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -713,7 +772,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection sqref="A1:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -733,7 +792,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>0.65641310661274999</v>
       </c>
       <c r="B2" s="3">
@@ -747,7 +806,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+      <c r="A3" s="3">
         <v>-0.100094132479392</v>
       </c>
       <c r="B3" s="3">
@@ -761,7 +820,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="A4" s="3">
         <v>0.51649063274268303</v>
       </c>
       <c r="B4" s="3">
@@ -775,7 +834,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="A5" s="3">
         <v>2.4314726829885398</v>
       </c>
       <c r="B5" s="3">
@@ -789,7 +848,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="A6" s="3">
         <v>-2.1032697392749098</v>
       </c>
       <c r="B6" s="3">
@@ -803,7 +862,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+      <c r="A7" s="3">
         <v>0.13191134233124199</v>
       </c>
       <c r="B7" s="3">
@@ -817,7 +876,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+      <c r="A8" s="3">
         <v>0.22969726655074801</v>
       </c>
       <c r="B8" s="3">
@@ -831,7 +890,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+      <c r="A9" s="3">
         <v>0.66256582258412799</v>
       </c>
       <c r="B9" s="3">
@@ -845,7 +904,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+      <c r="A10" s="3">
         <v>4.2401035574221098</v>
       </c>
       <c r="B10" s="3">
@@ -869,7 +928,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection sqref="A1:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -893,128 +952,128 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>2.41407382168491E-2</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>0.43429445069880901</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>0.66516231615465005</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>0.45042047532419399</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>6.7823578111430693E-2</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>0.86652434409406498</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>0.38861385318386898</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>0.453414412657064</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>-1.05383124192722E-2</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>-0.213770617850358</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>0.83123193924945804</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>0.44360989205885498</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>0.26521393468048798</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>1.4551368958659601</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>0.149271911004971</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>0.45643914027577998</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>0.248000224418404</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>1.3109490355139599</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>0.193364782994045</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>0.47262335166160102</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>1.6504170910705999E-2</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>0.56264701107270498</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>0.57513907552424703</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>0.45938691066764198</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>1.42821861086253E-2</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>1.1629686137124</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>0.248059077254769</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>0.43100115059602701</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>-0.16444517116044599</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>-1.45520843727225</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>0.14925215461721</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>0.43086867145624702</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>0.14379416678295801</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>0.74679518384034804</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>0.45722402012449498</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>0.44146324950031401</v>
       </c>
     </row>

</xml_diff>